<commit_message>
new schryver lcl data
Former-commit-id: cec67a4da2bcf09d693e78a96ef6962e8352eb1e
</commit_message>
<xml_diff>
--- a/db/dummydata/schryver/schryver__freight_rates.xlsx
+++ b/db/dummydata/schryver/schryver__freight_rates.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="45">
   <si>
     <t>CUSTOMER_ID</t>
   </si>
@@ -140,6 +140,15 @@
   <si>
     <t>Veracruz</t>
   </si>
+  <si>
+    <t>lcl</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>PER_WM</t>
+  </si>
 </sst>
 </file>
 
@@ -6281,18 +6290,138 @@
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="5"/>
-      <c r="F128" s="4"/>
-      <c r="G128" s="4"/>
+      <c r="D128" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E128" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F128" s="3">
+        <v>43285.0</v>
+      </c>
+      <c r="G128" s="4">
+        <v>43547.0</v>
+      </c>
+      <c r="H128" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I128" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J128" s="12">
+        <v>20.0</v>
+      </c>
+      <c r="K128" s="12">
+        <v>1000.0</v>
+      </c>
+      <c r="L128" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N128" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="O128" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P128" s="12">
+        <v>35.0</v>
+      </c>
+      <c r="Q128" s="12">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="5"/>
-      <c r="F129" s="4"/>
-      <c r="G129" s="4"/>
+      <c r="D129" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E129" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F129" s="3">
+        <v>43285.0</v>
+      </c>
+      <c r="G129" s="4">
+        <v>43547.0</v>
+      </c>
+      <c r="H129" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I129" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J129" s="12">
+        <v>20.0</v>
+      </c>
+      <c r="K129" s="12">
+        <v>1000.0</v>
+      </c>
+      <c r="L129" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M129" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N129" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="O129" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P129" s="12">
+        <v>35.0</v>
+      </c>
+      <c r="Q129" s="12">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="5"/>
-      <c r="F130" s="4"/>
-      <c r="G130" s="4"/>
+      <c r="D130" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E130" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F130" s="3">
+        <v>43285.0</v>
+      </c>
+      <c r="G130" s="4">
+        <v>43547.0</v>
+      </c>
+      <c r="H130" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I130" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J130" s="12">
+        <v>20.0</v>
+      </c>
+      <c r="K130" s="12">
+        <v>1000.0</v>
+      </c>
+      <c r="L130" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M130" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N130" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="O130" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P130" s="12">
+        <v>35.0</v>
+      </c>
+      <c r="Q130" s="12">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="5"/>

</xml_diff>